<commit_message>
Translate Bonuses and Other tabs
</commit_message>
<xml_diff>
--- a/i18n/nl.xlsx
+++ b/i18n/nl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matej\Programming\wingsearch\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erik.huizinga/Dropbox/Software/Repos/GitHub/navarog/wingsearch/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4038B88-5E1D-46C8-876E-AD0084B1CCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05D04ED-428F-924E-AD7C-3F950467FA2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="938">
   <si>
     <t>id</t>
   </si>
@@ -2532,6 +2532,330 @@
   </si>
   <si>
     <t>Geelgors</t>
+  </si>
+  <si>
+    <t>ALS GEACTIVEERD</t>
+  </si>
+  <si>
+    <t>ALS GESPEELD</t>
+  </si>
+  <si>
+    <t>EENMALIG TUSSEN BEURTEN</t>
+  </si>
+  <si>
+    <t>EINDE RONDE</t>
+  </si>
+  <si>
+    <t>van de kaarten</t>
+  </si>
+  <si>
+    <t>Wijnbouwer</t>
+  </si>
+  <si>
+    <t>Vogels die [fruit] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel met een [fruit]-symbool. De vogel mag daarnaast andere soorten voedsel eten.</t>
+  </si>
+  <si>
+    <t>2 of 3 vogels: 3[point]; 4+ vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Ecoloog</t>
+  </si>
+  <si>
+    <t>Aantal vogels ini je leefomgeving met de minste vogels</t>
+  </si>
+  <si>
+    <t>Bij een gellijke stand: heb je bijvoorbeeld in elke leefomgeving 3 vogels, dan bevat je leefomgeving met de minste vogels er 3.</t>
+  </si>
+  <si>
+    <t>Etholoog</t>
+  </si>
+  <si>
+    <t>In één leefomgevinig naar keuze:</t>
+  </si>
+  <si>
+    <t>(bijvoobeeld bruin, wit, roze, blauwgroen)\nVogels zonder eigenschap gelden als wit.</t>
+  </si>
+  <si>
+    <t>2[point] per vogel</t>
+  </si>
+  <si>
+    <t>2[point] per eigenschapskleur</t>
+  </si>
+  <si>
+    <t>Fotograaf</t>
+  </si>
+  <si>
+    <t>Vogels met kleuren in hun namen</t>
+  </si>
+  <si>
+    <t>Onder kleuren vallen azuur, blauw, bont, bruin, citroen, geel, goud, grijs, groen, indigo, lazuli, purper, robijn, rood, rosse, tweekleurig, wit, zilver, zwart.</t>
+  </si>
+  <si>
+    <t>4 of 5 vogels: 3[point]; 6+ vogels: 6[point]</t>
+  </si>
+  <si>
+    <t>Broedmanager</t>
+  </si>
+  <si>
+    <t>Vogels waarop ten minste 4 eieren liggen</t>
+  </si>
+  <si>
+    <t>1[point] per vogel</t>
+  </si>
+  <si>
+    <t>Visserijbeheerder</t>
+  </si>
+  <si>
+    <t>Vogels die [fish] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel met een [fish]-symbool. De vogel mag daarnaast andere soorten voedsel eten.</t>
+  </si>
+  <si>
+    <t>2 of 3 vogels: 3[point]; 4+ vogels: 8[point]</t>
+  </si>
+  <si>
+    <t>Voedselwebexpert</t>
+  </si>
+  <si>
+    <t>Vogels die uitsluitend [invertebrate] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel met een [invertebrate]-symbool en geen andere voedselsymbolen.</t>
+  </si>
+  <si>
+    <t>Dieetspecialist</t>
+  </si>
+  <si>
+    <t>Vogels met voedselkosten van 3 voedsel</t>
+  </si>
+  <si>
+    <t>2 - 3 vogels: 3[point]; 4+ vogels: 6[point]</t>
+  </si>
+  <si>
+    <t>Vogels met vleugelwijdten boven 65 cm</t>
+  </si>
+  <si>
+    <t>Kaartenmaker</t>
+  </si>
+  <si>
+    <t>Vogels met gebiedsgerelateerde termen in hun namen</t>
+  </si>
+  <si>
+    <t>Onder gebiedsgerelateerde namen vallen Amerikaans, Baltimore, berg, Californisch, Canadees, Carolina, Ĳslandse, Inca, Louisiana, Mexicaans, Mississippi, prairie, savannah, woestijn.</t>
+  </si>
+  <si>
+    <t>3 of 4 vogels: 4[point]; 5+ vogels: 8[point]</t>
+  </si>
+  <si>
+    <t>"Grote Vogel"-Specialist</t>
+  </si>
+  <si>
+    <t>Visionair Leider</t>
+  </si>
+  <si>
+    <t>Vogelkaarten in de hand aan het einde van het spel</t>
+  </si>
+  <si>
+    <t>5, 6 of 7 vogels: 4[point]; 8+ vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Historicus</t>
+  </si>
+  <si>
+    <t>Vogels die naar een persoon zijn vernoemd</t>
+  </si>
+  <si>
+    <t>Onder deze categorie vallen Anna's, Bairds, Bells, Bewicks, Brewers, Cassins, Clarks, Coopers, Forsters, Franklins, Gambels, Lincolns, Says, Stellers.</t>
+  </si>
+  <si>
+    <t>Platformbouwer</t>
+  </si>
+  <si>
+    <t>Vogels met [platform]-nesten</t>
+  </si>
+  <si>
+    <t>De vogels moeten een [platform]- of [star]-nestsymbool hebben.</t>
+  </si>
+  <si>
+    <t>4 of 5 vogels: 4[point]; 6+ vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Prairiebeheerder</t>
+  </si>
+  <si>
+    <t>Vogels die uitsluitend in [grassland] kunnen leven</t>
+  </si>
+  <si>
+    <t>Moeraswetenschapper</t>
+  </si>
+  <si>
+    <t>Vogels die uitsluitend in [wetland] kunnen leven</t>
+  </si>
+  <si>
+    <t>3 of 4 vogels: 3[point]; 5 vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Boswachter</t>
+  </si>
+  <si>
+    <t>Vogels die uitsluitend in [forest] kunnen leven</t>
+  </si>
+  <si>
+    <t>3 of 4 vogels: 4[point]; 5 vogels: 8[point]</t>
+  </si>
+  <si>
+    <t>Vogelteller</t>
+  </si>
+  <si>
+    <t>Vogels met een [focking]-eigenschap</t>
+  </si>
+  <si>
+    <t>Gedragswetenschapper</t>
+  </si>
+  <si>
+    <t>Voor elke kolom waarin vogels met eigenschappen in 3 verschillende kleuren liggen (bijvoorbeeld bruin, wit, roze, blauwgroen):</t>
+  </si>
+  <si>
+    <t>Vogels zonder eigenschap gelden als wit.</t>
+  </si>
+  <si>
+    <t>3[point] per kolom</t>
+  </si>
+  <si>
+    <t>Knaagdierenexpert</t>
+  </si>
+  <si>
+    <t>Vogels die [rodent] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel met een [rodent]-symbool. De vogel mag daarnaast andere soorten voedsel eten.</t>
+  </si>
+  <si>
+    <t>Allesetersdeskundige</t>
+  </si>
+  <si>
+    <t>Vogels die [wild] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel die een [wild]-symbool als onderdeel van zijn voedselkosten heeft.</t>
+  </si>
+  <si>
+    <t>Nestkastenbouwer</t>
+  </si>
+  <si>
+    <t>Vogels met [cavity]-nesten</t>
+  </si>
+  <si>
+    <t>De vogels moeten een [cavity]- of [star]-nestsymbool hebben.</t>
+  </si>
+  <si>
+    <t>Burgerwetenschapper</t>
+  </si>
+  <si>
+    <t>Vogels met weggestopte kaarten</t>
+  </si>
+  <si>
+    <t>4 - 6 vogels: 3[point]; 7+ vogels: 6[point]</t>
+  </si>
+  <si>
+    <t>Ontleedkundige</t>
+  </si>
+  <si>
+    <t>Vogels met lichaamsdelen in hun naam</t>
+  </si>
+  <si>
+    <t>Onder lichaamsdelen vallen been, bek, borst, buik, eikel, hals, kaak, keel, kop, oog, oor, schouder, snavel, staart, teen, vleugel.</t>
+  </si>
+  <si>
+    <t>Achtertuinvogelaar</t>
+  </si>
+  <si>
+    <t>Vogels die minder dan 4 punten waard zijn</t>
+  </si>
+  <si>
+    <t>5 of 6 vogels: 3[point], 7+ vogels: 6[point]</t>
+  </si>
+  <si>
+    <t>Vogelvoeder</t>
+  </si>
+  <si>
+    <t>Vogels die [seed] eten</t>
+  </si>
+  <si>
+    <t>Elke vogel met een [seed]-symbool. De vogel mag daarnaast andere soorten voedsel eten.</t>
+  </si>
+  <si>
+    <t>5, 6 of 7 vogels: 3[point]; 8+ vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Valkenier</t>
+  </si>
+  <si>
+    <t>Vogels met een [predator]-eigenschap</t>
+  </si>
+  <si>
+    <t>Vogelringer</t>
+  </si>
+  <si>
+    <t>Vogels die in meerdere leefomgevingen kunnen leven</t>
+  </si>
+  <si>
+    <t>4 - 5 vogels: 4[point]; 6+ vogels: 7[point]</t>
+  </si>
+  <si>
+    <t>Gebiedsomheiner</t>
+  </si>
+  <si>
+    <t>Vogels met [ground]-nesten</t>
+  </si>
+  <si>
+    <t>De vogels moeten een [ground]- of [star]-nestsymbool hebben.</t>
+  </si>
+  <si>
+    <t>Broedkundige</t>
+  </si>
+  <si>
+    <t>Vogels waar ten minste 1 ei op ligt</t>
+  </si>
+  <si>
+    <t>7 of 8 vogels: 3[point]; 9+ vogels: 6[point]</t>
+  </si>
+  <si>
+    <t>Zangvogelspecalist</t>
+  </si>
+  <si>
+    <t>Vogels met vleugelwijdten van 30 cm of minder</t>
+  </si>
+  <si>
+    <t>Heemtuinier</t>
+  </si>
+  <si>
+    <t>Vogels met [bowl]-nesten</t>
+  </si>
+  <si>
+    <t>De vogels moeten een [bowl]- of [star]-nestsymbool hebben.</t>
+  </si>
+  <si>
+    <t>Vogels die 3 of 4 punten waard zijn.</t>
+  </si>
+  <si>
+    <t>De Automa houdt er ten hoogste 2 (hogere waarde eerst).</t>
+  </si>
+  <si>
+    <t>[automa] Auvogelaar</t>
+  </si>
+  <si>
+    <t>[automa] RASPB Erelid</t>
+  </si>
+  <si>
+    <t>Vogels die 5, 6 of 7 punten waard zijn.</t>
+  </si>
+  <si>
+    <t>De Automa houdt er ten hoogste één (die met de hoogste waarde).</t>
   </si>
 </sst>
 </file>
@@ -2959,21 +3283,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D262"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.46484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2993,7 +3317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3013,7 +3337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3033,7 +3357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -3053,7 +3377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5</v>
       </c>
@@ -3073,7 +3397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
@@ -3093,7 +3417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -3113,7 +3437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -3133,7 +3457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -3153,7 +3477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -3173,7 +3497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3193,7 +3517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3213,7 +3537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -3233,7 +3557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -3253,7 +3577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -3273,7 +3597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -3293,7 +3617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
@@ -3313,7 +3637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
@@ -3333,7 +3657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
@@ -3353,7 +3677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -3373,7 +3697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
@@ -3393,7 +3717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
@@ -3413,7 +3737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
@@ -3433,7 +3757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
@@ -3453,7 +3777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
@@ -3473,7 +3797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -3493,7 +3817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
@@ -3513,7 +3837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -3533,7 +3857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -3553,7 +3877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -3573,7 +3897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3593,7 +3917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -3613,7 +3937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -3633,7 +3957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -3653,7 +3977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -3673,7 +3997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>36</v>
       </c>
@@ -3693,7 +4017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>37</v>
       </c>
@@ -3713,7 +4037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>38</v>
       </c>
@@ -3733,7 +4057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>39</v>
       </c>
@@ -3753,7 +4077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3773,7 +4097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>41</v>
       </c>
@@ -3793,7 +4117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>42</v>
       </c>
@@ -3813,7 +4137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>43</v>
       </c>
@@ -3833,7 +4157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>44</v>
       </c>
@@ -3853,7 +4177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>45</v>
       </c>
@@ -3873,7 +4197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>46</v>
       </c>
@@ -3893,7 +4217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>47</v>
       </c>
@@ -3913,7 +4237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>48</v>
       </c>
@@ -3933,7 +4257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>49</v>
       </c>
@@ -3953,7 +4277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>50</v>
       </c>
@@ -3973,7 +4297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>51</v>
       </c>
@@ -3993,7 +4317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>52</v>
       </c>
@@ -4013,7 +4337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>53</v>
       </c>
@@ -4033,7 +4357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>54</v>
       </c>
@@ -4053,7 +4377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>55</v>
       </c>
@@ -4073,7 +4397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>56</v>
       </c>
@@ -4093,7 +4417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>57</v>
       </c>
@@ -4113,7 +4437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>58</v>
       </c>
@@ -4133,7 +4457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>59</v>
       </c>
@@ -4153,7 +4477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>60</v>
       </c>
@@ -4173,7 +4497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>61</v>
       </c>
@@ -4193,7 +4517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>62</v>
       </c>
@@ -4213,7 +4537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>63</v>
       </c>
@@ -4233,7 +4557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>64</v>
       </c>
@@ -4253,7 +4577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>65</v>
       </c>
@@ -4273,7 +4597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>66</v>
       </c>
@@ -4293,7 +4617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>67</v>
       </c>
@@ -4313,7 +4637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>68</v>
       </c>
@@ -4333,7 +4657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>69</v>
       </c>
@@ -4353,7 +4677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>70</v>
       </c>
@@ -4373,7 +4697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4393,7 +4717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4413,7 +4737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4433,7 +4757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4453,7 +4777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4473,7 +4797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4493,7 +4817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4513,7 +4837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>78</v>
       </c>
@@ -4533,7 +4857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4553,7 +4877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4573,7 +4897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4593,7 +4917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4613,7 +4937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4633,7 +4957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4653,7 +4977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4673,7 +4997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4693,7 +5017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>87</v>
       </c>
@@ -4713,7 +5037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>88</v>
       </c>
@@ -4733,7 +5057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>89</v>
       </c>
@@ -4753,7 +5077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>90</v>
       </c>
@@ -4773,7 +5097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>91</v>
       </c>
@@ -4793,7 +5117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>92</v>
       </c>
@@ -4813,7 +5137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>93</v>
       </c>
@@ -4833,7 +5157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>94</v>
       </c>
@@ -4853,7 +5177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>95</v>
       </c>
@@ -4873,7 +5197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>96</v>
       </c>
@@ -4893,7 +5217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>97</v>
       </c>
@@ -4913,7 +5237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4933,7 +5257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4953,7 +5277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4973,7 +5297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>101</v>
       </c>
@@ -4993,7 +5317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>102</v>
       </c>
@@ -5013,7 +5337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>103</v>
       </c>
@@ -5033,7 +5357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>104</v>
       </c>
@@ -5053,7 +5377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>105</v>
       </c>
@@ -5073,7 +5397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>106</v>
       </c>
@@ -5093,7 +5417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>107</v>
       </c>
@@ -5113,7 +5437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>108</v>
       </c>
@@ -5133,7 +5457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>109</v>
       </c>
@@ -5153,7 +5477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>110</v>
       </c>
@@ -5173,7 +5497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>111</v>
       </c>
@@ -5193,7 +5517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>112</v>
       </c>
@@ -5213,7 +5537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>113</v>
       </c>
@@ -5233,7 +5557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>114</v>
       </c>
@@ -5253,7 +5577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>115</v>
       </c>
@@ -5273,7 +5597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5293,7 +5617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>117</v>
       </c>
@@ -5313,7 +5637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>118</v>
       </c>
@@ -5333,7 +5657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>119</v>
       </c>
@@ -5353,7 +5677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>120</v>
       </c>
@@ -5373,7 +5697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>121</v>
       </c>
@@ -5393,7 +5717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>122</v>
       </c>
@@ -5413,7 +5737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>123</v>
       </c>
@@ -5433,7 +5757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>124</v>
       </c>
@@ -5453,7 +5777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>125</v>
       </c>
@@ -5473,7 +5797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>126</v>
       </c>
@@ -5493,7 +5817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>127</v>
       </c>
@@ -5513,7 +5837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>128</v>
       </c>
@@ -5533,7 +5857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>129</v>
       </c>
@@ -5553,7 +5877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>130</v>
       </c>
@@ -5573,7 +5897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>131</v>
       </c>
@@ -5593,7 +5917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>132</v>
       </c>
@@ -5613,7 +5937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>133</v>
       </c>
@@ -5633,7 +5957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>134</v>
       </c>
@@ -5653,7 +5977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>135</v>
       </c>
@@ -5673,7 +5997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>136</v>
       </c>
@@ -5693,7 +6017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>137</v>
       </c>
@@ -5713,7 +6037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>138</v>
       </c>
@@ -5733,7 +6057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>139</v>
       </c>
@@ -5753,7 +6077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>140</v>
       </c>
@@ -5773,7 +6097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>141</v>
       </c>
@@ -5793,7 +6117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>142</v>
       </c>
@@ -5813,7 +6137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>143</v>
       </c>
@@ -5833,7 +6157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>144</v>
       </c>
@@ -5853,7 +6177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>145</v>
       </c>
@@ -5873,7 +6197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>146</v>
       </c>
@@ -5893,7 +6217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>147</v>
       </c>
@@ -5913,7 +6237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>148</v>
       </c>
@@ -5933,7 +6257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>149</v>
       </c>
@@ -5953,7 +6277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>150</v>
       </c>
@@ -5973,7 +6297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>151</v>
       </c>
@@ -5993,7 +6317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>152</v>
       </c>
@@ -6013,7 +6337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>153</v>
       </c>
@@ -6033,7 +6357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>154</v>
       </c>
@@ -6053,7 +6377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>155</v>
       </c>
@@ -6073,7 +6397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>156</v>
       </c>
@@ -6093,7 +6417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>157</v>
       </c>
@@ -6113,7 +6437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>158</v>
       </c>
@@ -6133,7 +6457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>159</v>
       </c>
@@ -6153,7 +6477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>160</v>
       </c>
@@ -6173,7 +6497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>161</v>
       </c>
@@ -6193,7 +6517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>162</v>
       </c>
@@ -6213,7 +6537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>163</v>
       </c>
@@ -6233,7 +6557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>164</v>
       </c>
@@ -6253,7 +6577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>165</v>
       </c>
@@ -6273,7 +6597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>166</v>
       </c>
@@ -6293,7 +6617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>167</v>
       </c>
@@ -6313,7 +6637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>168</v>
       </c>
@@ -6333,7 +6657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>169</v>
       </c>
@@ -6353,7 +6677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>170</v>
       </c>
@@ -6373,7 +6697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>171</v>
       </c>
@@ -6393,7 +6717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>172</v>
       </c>
@@ -6413,7 +6737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>173</v>
       </c>
@@ -6433,7 +6757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>174</v>
       </c>
@@ -6453,7 +6777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>175</v>
       </c>
@@ -6473,7 +6797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>176</v>
       </c>
@@ -6493,7 +6817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>177</v>
       </c>
@@ -6513,7 +6837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>178</v>
       </c>
@@ -6533,7 +6857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>179</v>
       </c>
@@ -6553,7 +6877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>180</v>
       </c>
@@ -6573,7 +6897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>181</v>
       </c>
@@ -6593,7 +6917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>182</v>
       </c>
@@ -6613,7 +6937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>183</v>
       </c>
@@ -6633,7 +6957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>184</v>
       </c>
@@ -6653,7 +6977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>185</v>
       </c>
@@ -6673,7 +6997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>186</v>
       </c>
@@ -6693,7 +7017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>187</v>
       </c>
@@ -6713,7 +7037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>188</v>
       </c>
@@ -6733,7 +7057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>189</v>
       </c>
@@ -6753,7 +7077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>190</v>
       </c>
@@ -6773,7 +7097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>191</v>
       </c>
@@ -6793,7 +7117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>192</v>
       </c>
@@ -6813,7 +7137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>193</v>
       </c>
@@ -6833,7 +7157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>194</v>
       </c>
@@ -6853,7 +7177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>195</v>
       </c>
@@ -6873,7 +7197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>196</v>
       </c>
@@ -6893,7 +7217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>197</v>
       </c>
@@ -6913,7 +7237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>198</v>
       </c>
@@ -6933,7 +7257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>199</v>
       </c>
@@ -6953,7 +7277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>200</v>
       </c>
@@ -6973,7 +7297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>201</v>
       </c>
@@ -6993,7 +7317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>203</v>
       </c>
@@ -7013,7 +7337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>204</v>
       </c>
@@ -7033,7 +7357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>205</v>
       </c>
@@ -7053,7 +7377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>206</v>
       </c>
@@ -7073,7 +7397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>207</v>
       </c>
@@ -7093,7 +7417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>208</v>
       </c>
@@ -7113,7 +7437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>209</v>
       </c>
@@ -7133,7 +7457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>210</v>
       </c>
@@ -7153,7 +7477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>211</v>
       </c>
@@ -7173,7 +7497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>212</v>
       </c>
@@ -7193,7 +7517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>213</v>
       </c>
@@ -7213,7 +7537,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>214</v>
       </c>
@@ -7233,7 +7557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>215</v>
       </c>
@@ -7253,7 +7577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>216</v>
       </c>
@@ -7273,7 +7597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>217</v>
       </c>
@@ -7293,7 +7617,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>218</v>
       </c>
@@ -7313,7 +7637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>219</v>
       </c>
@@ -7333,7 +7657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>220</v>
       </c>
@@ -7353,7 +7677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>221</v>
       </c>
@@ -7373,7 +7697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>222</v>
       </c>
@@ -7393,7 +7717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>223</v>
       </c>
@@ -7413,7 +7737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>224</v>
       </c>
@@ -7433,7 +7757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>225</v>
       </c>
@@ -7453,7 +7777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>226</v>
       </c>
@@ -7473,7 +7797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>227</v>
       </c>
@@ -7493,7 +7817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>228</v>
       </c>
@@ -7513,7 +7837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>229</v>
       </c>
@@ -7533,7 +7857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>230</v>
       </c>
@@ -7553,7 +7877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>231</v>
       </c>
@@ -7573,7 +7897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>232</v>
       </c>
@@ -7593,7 +7917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>233</v>
       </c>
@@ -7613,7 +7937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>234</v>
       </c>
@@ -7633,7 +7957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>235</v>
       </c>
@@ -7653,7 +7977,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>236</v>
       </c>
@@ -7673,7 +7997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>237</v>
       </c>
@@ -7693,7 +8017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>238</v>
       </c>
@@ -7713,7 +8037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>239</v>
       </c>
@@ -7733,7 +8057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>240</v>
       </c>
@@ -7753,7 +8077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>241</v>
       </c>
@@ -7773,7 +8097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>242</v>
       </c>
@@ -7793,7 +8117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>243</v>
       </c>
@@ -7813,7 +8137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>244</v>
       </c>
@@ -7833,7 +8157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>245</v>
       </c>
@@ -7853,7 +8177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>246</v>
       </c>
@@ -7873,7 +8197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>247</v>
       </c>
@@ -7893,7 +8217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>248</v>
       </c>
@@ -7913,7 +8237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>249</v>
       </c>
@@ -7933,7 +8257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>250</v>
       </c>
@@ -7953,7 +8277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>251</v>
       </c>
@@ -7973,7 +8297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>252</v>
       </c>
@@ -7993,7 +8317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>253</v>
       </c>
@@ -8013,7 +8337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>254</v>
       </c>
@@ -8033,7 +8357,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>255</v>
       </c>
@@ -8053,7 +8377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>256</v>
       </c>
@@ -8073,7 +8397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>257</v>
       </c>
@@ -8093,7 +8417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>258</v>
       </c>
@@ -8113,7 +8437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>259</v>
       </c>
@@ -8133,7 +8457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>260</v>
       </c>
@@ -8153,7 +8477,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>261</v>
       </c>
@@ -8173,7 +8497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>262</v>
       </c>
@@ -8193,7 +8517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>263</v>
       </c>
@@ -8225,20 +8549,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29F73C7-BAF7-4DDB-A3F3-74A889132A9F}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="118" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8261,7 +8587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -8269,22 +8595,22 @@
         <v>533</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>906</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>907</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>908</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>838</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -8292,22 +8618,22 @@
         <v>534</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>909</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>910</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>911</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -8315,22 +8641,22 @@
         <v>535</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>890</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>891</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>892</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>893</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -8338,22 +8664,22 @@
         <v>536</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>918</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>919</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>920</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -8361,22 +8687,22 @@
         <v>537</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>888</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>889</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1005</v>
       </c>
@@ -8384,22 +8710,22 @@
         <v>538</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>912</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>913</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>914</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>8</v>
+        <v>915</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1006</v>
       </c>
@@ -8407,22 +8733,22 @@
         <v>539</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>851</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>852</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>8</v>
+        <v>853</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1007</v>
       </c>
@@ -8430,22 +8756,22 @@
         <v>540</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>8</v>
+        <v>865</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>866</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>867</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>8</v>
+        <v>868</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1008</v>
       </c>
@@ -8453,22 +8779,22 @@
         <v>541</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>903</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>904</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>8</v>
+        <v>905</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1009</v>
       </c>
@@ -8476,22 +8802,22 @@
         <v>542</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>861</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
+        <v>862</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>8</v>
+        <v>863</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1010</v>
       </c>
@@ -8499,22 +8825,22 @@
         <v>543</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>839</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>840</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>841</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1011</v>
       </c>
@@ -8522,22 +8848,22 @@
         <v>544</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>8</v>
+        <v>921</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>922</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>923</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>8</v>
+        <v>879</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1012</v>
       </c>
@@ -8545,22 +8871,22 @@
         <v>545</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>842</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>843</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>844</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
+        <v>846</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1013</v>
       </c>
@@ -8568,22 +8894,22 @@
         <v>546</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
+        <v>916</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>8</v>
+        <v>917</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1014</v>
       </c>
@@ -8591,22 +8917,22 @@
         <v>547</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
+        <v>854</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>8</v>
+        <v>855</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
+        <v>856</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>8</v>
+        <v>857</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1015</v>
       </c>
@@ -8614,22 +8940,22 @@
         <v>548</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>8</v>
+        <v>858</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>859</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>8</v>
+        <v>860</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1016</v>
       </c>
@@ -8637,22 +8963,22 @@
         <v>549</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>885</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>8</v>
+        <v>886</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>8</v>
+        <v>887</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1017</v>
       </c>
@@ -8660,22 +8986,22 @@
         <v>550</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>873</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>8</v>
+        <v>874</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
+        <v>875</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1018</v>
       </c>
@@ -8683,22 +9009,22 @@
         <v>551</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>869</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>864</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>8</v>
+        <v>850</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1019</v>
       </c>
@@ -8706,22 +9032,22 @@
         <v>552</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>8</v>
+        <v>900</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>8</v>
+        <v>901</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>902</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>8</v>
+        <v>879</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1020</v>
       </c>
@@ -8729,22 +9055,22 @@
         <v>553</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>8</v>
+        <v>897</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>8</v>
+        <v>898</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>8</v>
+        <v>899</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1021</v>
       </c>
@@ -8752,22 +9078,22 @@
         <v>554</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>924</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>8</v>
+        <v>925</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>8</v>
+        <v>926</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1022</v>
       </c>
@@ -8775,22 +9101,22 @@
         <v>555</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
+        <v>927</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>928</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>8</v>
+        <v>850</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1023</v>
       </c>
@@ -8798,22 +9124,22 @@
         <v>556</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>8</v>
+        <v>847</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>848</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>8</v>
+        <v>849</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>8</v>
+        <v>850</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1024</v>
       </c>
@@ -8821,22 +9147,22 @@
         <v>557</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>8</v>
+        <v>876</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>8</v>
+        <v>877</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>8</v>
+        <v>878</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>8</v>
+        <v>879</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1025</v>
       </c>
@@ -8844,22 +9170,22 @@
         <v>558</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>8</v>
+        <v>880</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>8</v>
+        <v>881</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>8</v>
+        <v>857</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1026</v>
       </c>
@@ -8867,22 +9193,22 @@
         <v>559</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>8</v>
+        <v>894</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>8</v>
+        <v>895</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>8</v>
+        <v>896</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>845</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1027</v>
       </c>
@@ -8890,22 +9216,22 @@
         <v>560</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>8</v>
+        <v>870</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>871</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>8</v>
+        <v>872</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1028</v>
       </c>
@@ -8913,22 +9239,22 @@
         <v>561</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>8</v>
+        <v>835</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>8</v>
+        <v>836</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>8</v>
+        <v>837</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>8</v>
+        <v>838</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1029</v>
       </c>
@@ -8936,22 +9262,22 @@
         <v>562</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>8</v>
+        <v>882</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>8</v>
+        <v>883</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>8</v>
+        <v>884</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1030</v>
       </c>
@@ -8959,22 +9285,22 @@
         <v>563</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>8</v>
+        <v>929</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>8</v>
+        <v>930</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>8</v>
+        <v>931</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>8</v>
+        <v>879</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1031</v>
       </c>
@@ -8982,13 +9308,13 @@
         <v>564</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>8</v>
+        <v>934</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>8</v>
+        <v>932</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>8</v>
+        <v>933</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>8</v>
@@ -8997,7 +9323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1032</v>
       </c>
@@ -9005,13 +9331,13 @@
         <v>565</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>8</v>
+        <v>935</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>8</v>
+        <v>936</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>8</v>
+        <v>937</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>8</v>
@@ -9033,16 +9359,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.9296875" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9050,29 +9376,44 @@
         <v>566</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>571</v>
+      </c>
+      <c r="B6" t="s">
+        <v>834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dutch bird translations
</commit_message>
<xml_diff>
--- a/i18n/nl.xlsx
+++ b/i18n/nl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erik.huizinga/Dropbox/Software/Repos/GitHub/navarog/wingsearch/i18n/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F340B01-BE3D-704E-B4C6-514B58B32E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467B7A4D-2145-3440-B30D-8FEC16F9A061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="1062">
   <si>
     <t>id</t>
   </si>
@@ -2459,9 +2459,6 @@
     <t>Roodkopgier</t>
   </si>
   <si>
-    <t>Vauxâ€™ gierzwaluw</t>
-  </si>
-  <si>
     <t>Groene zwaluw</t>
   </si>
   <si>
@@ -2927,15 +2924,9 @@
     <t>herhaal een bruine eigenschap van een andere vogel in deze leefomgeving.</t>
   </si>
   <si>
-    <t>all spelers trekken 1 [card] van de gedekte stapel.</t>
-  </si>
-  <si>
     <t>leg ten hoogste 5 [wild] uit je voorraad af. Stop voor elk ervan 1 [card] van de gedekte stapel onder deze vogel weg.</t>
   </si>
   <si>
-    <t>voor elke [rodent] in de kosten van deze vogel mag je in plaats daarvan 1 [card] ui je hand betalen. Doe je dat, stop de betaalde [card] dan onder deze kaart weg.</t>
-  </si>
-  <si>
     <t>gooi alle dobbelstenen opnieuw in het vogelhuisje. Doe je dat, dan pak je daarna 1 [invertebrate] uit het vogelhuisje.</t>
   </si>
   <si>
@@ -3045,6 +3036,198 @@
   </si>
   <si>
     <t>leg 1 [card] uit je hand af. Doe je dat, speel dan nog een vogel in je [forest]. Betaal de gebruikelijke voedsel- en eikosten.</t>
+  </si>
+  <si>
+    <t>alle spelers pakken 1 [fish] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>als een andere speler om welke reden dan ook een [card] wegstopt, stop dan 1 [card] van de gedekte stapel onder deze vogel weg.</t>
+  </si>
+  <si>
+    <t>stop een [card] uit je hand onder deze vogel weg. Doe je dat, pak dan 1 [fruit] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>Vaux' gierzwaluw</t>
+  </si>
+  <si>
+    <t>als een [predator] van een andere speler lukt, pak jij 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>leg 1 [seed] uit je voorraad af. Doe je dat, leg dan 2 [egg] op deze vogel.</t>
+  </si>
+  <si>
+    <t>leg 1 [seed] af om 2 [card] van de gedekte stapel onder deze vogel weg te stoppen.</t>
+  </si>
+  <si>
+    <t>pak 1 [seed] uit de voorraad en bewaar die op deze kaart.</t>
+  </si>
+  <si>
+    <t>trek zoveel [card] als het aantal spelers + 1. Te beginnen bij jou en daarna met de klok mee, kiest iedere speler 1 van deze kaarten en doet die in zijn hand. Jij houdt de overgebleven kaart.</t>
+  </si>
+  <si>
+    <t>leg 1 [egg] op deze vogel.</t>
+  </si>
+  <si>
+    <t>pak 1 [invertebrate] of [fruit] uit het vogelhuisje, indien beschikbaar.</t>
+  </si>
+  <si>
+    <t>pak 1 [invertebrate] uit het vogelhuisje, indien beschikbaar.</t>
+  </si>
+  <si>
+    <t>leg alle resterende open [card] af en vul de vogelhouder aan. Doe je dat, trek dan 1 van de nieuwe open [card].</t>
+  </si>
+  <si>
+    <t>pak 1 [seed] of [fruit] uit het vogelhuisje, indien beschikbaar.</t>
+  </si>
+  <si>
+    <t>pak 1 [invertebrate] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>de speler(s) met de minste [forest]-vogels pakt/pakken 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>trek 2 [card] van de gedekte stapel. Stop er 1 van onder deze vogel weg en hou de andere.</t>
+  </si>
+  <si>
+    <t>de speler(s) met de minste [wetland]-vogels: trek 1 [card].</t>
+  </si>
+  <si>
+    <t>als een andere speler de actie "Eieren leggen" uitvoert, legt deze vogel 1 [egg] op een andere vogel met een [bowl]-nest.</t>
+  </si>
+  <si>
+    <t>voor elke [rodent] in de kosten van deze vogel mag je in plaats daarvan 1 [card] uit je hand betalen. Doe je dat, stop de betaalde [card] dan onder deze kaart weg.</t>
+  </si>
+  <si>
+    <t>pak 3 [seed] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>alle spelers pakken 1 [seed] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>pak 1 [wild] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>leg 1 [egg] van één van je andere vogels af om 2 [wild] uit de voorraad te pakken.</t>
+  </si>
+  <si>
+    <t>als een andere speler de "pak voedsel"-actie uitvoert, pak dan aan het einde van zijn beurt 1 [invertebrate] of [fruit] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>leg 1 [egg] op elk van je vogels met een [platform]-nest.</t>
+  </si>
+  <si>
+    <t>werp alle dobbelstenen die niet in het vogelhuisje liggen. Pak zoveel [fish] uit de voorraad als je hebt geworpen en bewaar die op deze vogel.</t>
+  </si>
+  <si>
+    <t>steel 1 [wild] uit de voorraad van een andere speler en doe het in je persoonlijke voorraad. Hij pakt 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>als een andere speler de "pak voedsel"-actie uitvoert, pak dan aan het einde van zijn beurt 1 [seed] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>leg deze vogel horizontaal neer, zodat deze 2 [forest]-velden bedekt. Betaal de lagere eikosten.</t>
+  </si>
+  <si>
+    <t>trek 2 [card]. Iedere andere speler trekt 1 [card] van de gedekte stapel.</t>
+  </si>
+  <si>
+    <t>gooi alle dobbelstenen opnieuw in het vogelhuisje. Doe je dat, dan pak je daarna 1 [seed] of 1 [fruit] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>pak 1 [seed] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>kies 1 andere speler. Bewaar voor elke actiesteen op zijn [grassland] 1 [wild] uit de voorraad op één van je vogels.</t>
+  </si>
+  <si>
+    <t>alle spelers leggen 1 [egg] op een [ground]-vogel naar keuze. Jij mag daarnaast nog 1 [egg] op 1 andere [ground]-vogel naar keuze leggen.</t>
+  </si>
+  <si>
+    <t>pak alle [invertebrate] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>kies 1 andere speler. Voor elke actiesteen die hij op zijn [wetland] heeft, stop je 1 [card] uit je hand onder deze vogel weg. Trek dan hetzelfde aantal [card].</t>
+  </si>
+  <si>
+    <t>leg 1 [egg] op elk van je vogels met een [bowl]-nest.</t>
+  </si>
+  <si>
+    <t>leg ten hoogste 5 [seed] uit je voorraad af. Stop voor elk ervan 1 [card] van de gedekte stapel onder deze vogel weg.</t>
+  </si>
+  <si>
+    <t>pak 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>gooi alle dobbelstenen opnieuw in het vogelhuisje. Doe je dat, dan pak je daarna 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>steel 1 [seed] uit de voorraad van een andere speler en bewaar het op deze kaart. Hij pakt 1 [die] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>als deze vogel aan de voorwaarden van het "Einde ronde"-doel voldoet, telt hij dubbel.</t>
+  </si>
+  <si>
+    <t>pak alle [fish] die in het vogelhuisje liggen.</t>
+  </si>
+  <si>
+    <t>trek 2 [card].</t>
+  </si>
+  <si>
+    <t>kies 1–5 vogels in deze leefomgeving. Stop 1 [card] uit je hand onder elk ervan weg.</t>
+  </si>
+  <si>
+    <t>bekijk een [card] van de gedekte stapel. Is die &lt; 50 cm, stop hem dan weg onder deze kaart. Zo niet, leg hem dan af.</t>
+  </si>
+  <si>
+    <t>als een andere speler de "leg eieren"-actie uitvoert, legt deze vogel 1 [egg] op een andere vogel met een [bowl]- of [ground] nest.</t>
+  </si>
+  <si>
+    <t>als een andere speler de actie "Voedsel pakken" uitvoert en ten minste 1 [rodent] pakt, dan pak jij ook 1 [rodent] en bewaar je die op deze kaart.</t>
+  </si>
+  <si>
+    <t>kies een leefomgeving zonder [egg]. Leg 1 [egg] op elke vogel in die leefomgeving.</t>
+  </si>
+  <si>
+    <t>pak 1 [fruit] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>leg ten hoogste 5 [invertebrate] uit je voorraad af. Stop voor elk ervan 1 [card] van de gedekte stapel onder deze vogel weg.</t>
+  </si>
+  <si>
+    <t>speel een tweede vogel in je [wetland]. Betaal de normale kosten ervan.</t>
+  </si>
+  <si>
+    <t>stop een [card] uit je hand onder deze vogel weg. Doe je dat, leg dan 1 [egg] op een vogel naar keuze.</t>
+  </si>
+  <si>
+    <t>als een andere speler een [grassland]-vogel speelt, stop jij een [card] uit je hand weg onder deze vogel.</t>
+  </si>
+  <si>
+    <t>kies 1–3 vogels in je [wetland]. Stop onder elk ervan 1 [card] weg. Stop je ten minste 1 kaart weg, trek dan 1 [card].</t>
+  </si>
+  <si>
+    <t>verwijder 1 [die] naar keuze uit het vogelhuisje. Pak dan 1 [seed] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>gooi alle dobbelstenen opnieuw in het vogelhuisje. Doe je dat, dan pak je daarna 1 [seed] uit het vogelhuisje.</t>
+  </si>
+  <si>
+    <t>alle spelers leggen 1 [egg] op een [cavity]-vogel naar keuze. Jij mag daarnaast nog 1 [egg] op 1 andere [cavity]-vogel naar keuze leggen.</t>
+  </si>
+  <si>
+    <t>pak 3 [fish] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>leg 1 [fish] af om 2 [card] van de gedekte stapel onder deze vogel weg te stoppen.</t>
+  </si>
+  <si>
+    <t>pak 1 open [card] die in [wetland] kan leven.</t>
+  </si>
+  <si>
+    <t>stop een [card] uit je hand onder deze vogel weg. Doe je dat, pak dan 1 [invertebrate] of [seed] uit de voorraad.</t>
+  </si>
+  <si>
+    <t>trek 1 nieuwe bonuskaart. Trek dan 1 [die] uit het vogelhuisje.</t>
   </si>
 </sst>
 </file>
@@ -3475,8 +3658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3485,8 +3668,8 @@
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="138" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="141.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3523,7 +3706,7 @@
         <v>758</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>961</v>
+        <v>978</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -3543,7 +3726,7 @@
         <v>699</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>1050</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -3563,7 +3746,7 @@
         <v>579</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>1006</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -3583,7 +3766,7 @@
         <v>605</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>1002</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -3623,7 +3806,7 @@
         <v>731</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>1046</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -3643,7 +3826,7 @@
         <v>790</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
@@ -3663,7 +3846,7 @@
         <v>573</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -3683,7 +3866,7 @@
         <v>576</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
@@ -3703,7 +3886,7 @@
         <v>575</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>936</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -3723,7 +3906,7 @@
         <v>657</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -3743,7 +3926,7 @@
         <v>703</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -3763,7 +3946,7 @@
         <v>794</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>978</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -3783,7 +3966,7 @@
         <v>580</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>1020</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
@@ -3803,7 +3986,7 @@
         <v>600</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
+        <v>987</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -3823,7 +4006,7 @@
         <v>584</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>8</v>
+        <v>987</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
@@ -3843,7 +4026,7 @@
         <v>609</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>8</v>
+        <v>1042</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
@@ -3863,7 +4046,7 @@
         <v>578</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
+        <v>988</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
@@ -3880,10 +4063,10 @@
         <v>510</v>
       </c>
       <c r="D20" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>978</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>8</v>
@@ -3903,7 +4086,7 @@
         <v>590</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>1041</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>8</v>
@@ -3923,7 +4106,7 @@
         <v>585</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>8</v>
@@ -3943,7 +4126,7 @@
         <v>712</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>8</v>
+        <v>1055</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -3963,7 +4146,7 @@
         <v>588</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>8</v>
+        <v>1014</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -3983,7 +4166,7 @@
         <v>637</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
@@ -4003,7 +4186,7 @@
         <v>589</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
@@ -4023,7 +4206,7 @@
         <v>591</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>8</v>
@@ -4043,7 +4226,7 @@
         <v>597</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>8</v>
@@ -4063,7 +4246,7 @@
         <v>596</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>8</v>
@@ -4083,7 +4266,7 @@
         <v>737</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>8</v>
+        <v>942</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>8</v>
@@ -4103,7 +4286,7 @@
         <v>598</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
@@ -4123,7 +4306,7 @@
         <v>685</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>8</v>
@@ -4143,7 +4326,7 @@
         <v>616</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>8</v>
+        <v>971</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>8</v>
@@ -4163,7 +4346,7 @@
         <v>612</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>8</v>
@@ -4203,7 +4386,7 @@
         <v>746</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>8</v>
@@ -4243,7 +4426,7 @@
         <v>614</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>8</v>
+        <v>1012</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>8</v>
@@ -4283,7 +4466,7 @@
         <v>97</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>8</v>
@@ -4320,10 +4503,10 @@
         <v>502</v>
       </c>
       <c r="D42" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>8</v>
+        <v>1051</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
@@ -4343,7 +4526,7 @@
         <v>714</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>8</v>
@@ -4363,7 +4546,7 @@
         <v>682</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>8</v>
@@ -4383,7 +4566,7 @@
         <v>788</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>8</v>
@@ -4423,7 +4606,7 @@
         <v>678</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>8</v>
@@ -4463,7 +4646,7 @@
         <v>727</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>8</v>
+        <v>1047</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>8</v>
@@ -4483,7 +4666,7 @@
         <v>620</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>8</v>
@@ -4503,7 +4686,7 @@
         <v>619</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>8</v>
+        <v>938</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>8</v>
@@ -4523,7 +4706,7 @@
         <v>651</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>8</v>
@@ -4543,7 +4726,7 @@
         <v>622</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>8</v>
+        <v>1057</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>8</v>
@@ -4583,7 +4766,7 @@
         <v>647</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>8</v>
+        <v>977</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>8</v>
@@ -4623,7 +4806,7 @@
         <v>628</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>8</v>
+        <v>1007</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>8</v>
@@ -4663,7 +4846,7 @@
         <v>782</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>8</v>
+        <v>1004</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>8</v>
@@ -4680,10 +4863,10 @@
         <v>514</v>
       </c>
       <c r="D60" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>8</v>
+        <v>956</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>8</v>
@@ -4703,7 +4886,7 @@
         <v>631</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>8</v>
+        <v>1005</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>8</v>
@@ -4723,7 +4906,7 @@
         <v>632</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>8</v>
+        <v>1042</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>8</v>
@@ -4743,7 +4926,7 @@
         <v>635</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>8</v>
@@ -4763,7 +4946,7 @@
         <v>634</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>8</v>
@@ -4783,7 +4966,7 @@
         <v>636</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>8</v>
+        <v>1000</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>8</v>
@@ -4802,9 +4985,7 @@
       <c r="D66" t="s">
         <v>638</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
         <v>8</v>
       </c>
@@ -4843,7 +5024,7 @@
         <v>643</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>8</v>
+        <v>940</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>8</v>
@@ -4863,7 +5044,7 @@
         <v>663</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>8</v>
@@ -4883,7 +5064,7 @@
         <v>664</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>8</v>
+        <v>1061</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>8</v>
@@ -4923,7 +5104,7 @@
         <v>199</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>8</v>
+        <v>938</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>8</v>
@@ -4943,7 +5124,7 @@
         <v>754</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>8</v>
@@ -4963,7 +5144,7 @@
         <v>667</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>8</v>
@@ -4983,7 +5164,7 @@
         <v>760</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>8</v>
+        <v>1060</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>8</v>
@@ -5003,7 +5184,7 @@
         <v>572</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>8</v>
+        <v>966</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>8</v>
@@ -5023,7 +5204,7 @@
         <v>680</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>8</v>
+        <v>1031</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>8</v>
@@ -5043,7 +5224,7 @@
         <v>674</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>8</v>
@@ -5063,7 +5244,7 @@
         <v>774</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>8</v>
@@ -5083,7 +5264,7 @@
         <v>705</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>8</v>
+        <v>1034</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>8</v>
@@ -5103,7 +5284,7 @@
         <v>693</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>8</v>
@@ -5143,7 +5324,7 @@
         <v>701</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>8</v>
+        <v>976</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>8</v>
@@ -5163,7 +5344,7 @@
         <v>679</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>8</v>
+        <v>1039</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>8</v>
@@ -5200,10 +5381,10 @@
         <v>522</v>
       </c>
       <c r="D86" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>8</v>
@@ -5220,7 +5401,7 @@
         <v>518</v>
       </c>
       <c r="D87" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>8</v>
@@ -5240,10 +5421,10 @@
         <v>528</v>
       </c>
       <c r="D88" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>8</v>
@@ -5260,10 +5441,10 @@
         <v>484</v>
       </c>
       <c r="D89" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>8</v>
+        <v>1032</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>8</v>
@@ -5280,7 +5461,7 @@
         <v>524</v>
       </c>
       <c r="D90" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>8</v>
@@ -5300,10 +5481,10 @@
         <v>520</v>
       </c>
       <c r="D91" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>8</v>
+        <v>1016</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
@@ -5323,7 +5504,7 @@
         <v>666</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>8</v>
+        <v>1058</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>8</v>
@@ -5343,7 +5524,7 @@
         <v>786</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>8</v>
+        <v>1007</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>8</v>
@@ -5363,7 +5544,7 @@
         <v>594</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>8</v>
@@ -5383,7 +5564,7 @@
         <v>793</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>8</v>
@@ -5403,7 +5584,7 @@
         <v>795</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>8</v>
+        <v>1030</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>8</v>
@@ -5423,7 +5604,7 @@
         <v>662</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>8</v>
+        <v>956</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>8</v>
@@ -5443,7 +5624,7 @@
         <v>661</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>8</v>
+        <v>1049</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>8</v>
@@ -5463,7 +5644,7 @@
         <v>652</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>8</v>
@@ -5483,7 +5664,7 @@
         <v>743</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>8</v>
@@ -5503,7 +5684,7 @@
         <v>695</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>8</v>
@@ -5523,7 +5704,7 @@
         <v>577</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>8</v>
+        <v>1018</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>8</v>
@@ -5543,7 +5724,7 @@
         <v>624</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>8</v>
+        <v>1029</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>8</v>
@@ -5563,7 +5744,7 @@
         <v>710</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>8</v>
+        <v>1040</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>8</v>
@@ -5583,7 +5764,7 @@
         <v>736</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>8</v>
+        <v>977</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>8</v>
@@ -5603,7 +5784,7 @@
         <v>764</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>8</v>
@@ -5623,7 +5804,7 @@
         <v>586</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>8</v>
@@ -5663,7 +5844,7 @@
         <v>644</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>8</v>
@@ -5683,7 +5864,7 @@
         <v>708</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>8</v>
@@ -5720,10 +5901,10 @@
         <v>482</v>
       </c>
       <c r="D112" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>8</v>
@@ -5743,7 +5924,7 @@
         <v>629</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>8</v>
+        <v>1004</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>8</v>
@@ -5763,7 +5944,7 @@
         <v>752</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>8</v>
+        <v>1054</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>8</v>
@@ -5783,7 +5964,7 @@
         <v>700</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>8</v>
+        <v>1009</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>8</v>
@@ -5803,7 +5984,7 @@
         <v>707</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>8</v>
+        <v>1044</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>8</v>
@@ -5823,7 +6004,7 @@
         <v>630</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>8</v>
@@ -5843,7 +6024,7 @@
         <v>655</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>8</v>
@@ -5863,7 +6044,7 @@
         <v>702</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>8</v>
+        <v>1050</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>8</v>
@@ -5883,7 +6064,7 @@
         <v>610</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>8</v>
+        <v>941</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>8</v>
@@ -5903,7 +6084,7 @@
         <v>745</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>8</v>
+        <v>1017</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>8</v>
@@ -5923,7 +6104,7 @@
         <v>617</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>963</v>
+        <v>1017</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>8</v>
@@ -5963,7 +6144,7 @@
         <v>713</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>8</v>
+        <v>1013</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>8</v>
@@ -5983,7 +6164,7 @@
         <v>625</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>8</v>
+        <v>988</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>8</v>
@@ -6003,7 +6184,7 @@
         <v>719</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>8</v>
+        <v>1036</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>8</v>
@@ -6023,7 +6204,7 @@
         <v>654</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>8</v>
+        <v>1015</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>8</v>
@@ -6043,7 +6224,7 @@
         <v>595</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>8</v>
@@ -6060,7 +6241,7 @@
         <v>172</v>
       </c>
       <c r="D129" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
@@ -6081,7 +6262,7 @@
         <v>721</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>8</v>
+        <v>1023</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>8</v>
@@ -6101,7 +6282,7 @@
         <v>722</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>8</v>
+        <v>1008</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>8</v>
@@ -6121,7 +6302,7 @@
         <v>744</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>8</v>
+        <v>1024</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>8</v>
@@ -6138,7 +6319,7 @@
         <v>516</v>
       </c>
       <c r="D133" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>8</v>
@@ -6158,7 +6339,7 @@
         <v>506</v>
       </c>
       <c r="D134" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>8</v>
@@ -6181,7 +6362,7 @@
         <v>763</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>8</v>
@@ -6201,7 +6382,7 @@
         <v>698</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>8</v>
@@ -6221,7 +6402,7 @@
         <v>670</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>963</v>
+        <v>1017</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>8</v>
@@ -6261,7 +6442,7 @@
         <v>592</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>8</v>
@@ -6301,7 +6482,7 @@
         <v>729</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>8</v>
@@ -6321,7 +6502,7 @@
         <v>740</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>8</v>
+        <v>1053</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>8</v>
@@ -6341,7 +6522,7 @@
         <v>650</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>8</v>
+        <v>1045</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>8</v>
@@ -6361,7 +6542,7 @@
         <v>768</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>8</v>
@@ -6381,7 +6562,7 @@
         <v>715</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>8</v>
@@ -6401,7 +6582,7 @@
         <v>608</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>8</v>
+        <v>1025</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>8</v>
@@ -6421,7 +6602,7 @@
         <v>725</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>8</v>
@@ -6441,7 +6622,7 @@
         <v>671</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>8</v>
@@ -6461,7 +6642,7 @@
         <v>704</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>8</v>
+        <v>1038</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>8</v>
@@ -6481,7 +6662,7 @@
         <v>761</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>8</v>
+        <v>1019</v>
       </c>
       <c r="F150" s="1" t="s">
         <v>8</v>
@@ -6501,7 +6682,7 @@
         <v>607</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="F151" s="1" t="s">
         <v>8</v>
@@ -6521,7 +6702,7 @@
         <v>726</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="F152" s="1" t="s">
         <v>8</v>
@@ -6558,10 +6739,10 @@
         <v>486</v>
       </c>
       <c r="D154" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>8</v>
+        <v>1008</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>8</v>
@@ -6581,7 +6762,7 @@
         <v>646</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>8</v>
+        <v>1027</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>8</v>
@@ -6601,7 +6782,7 @@
         <v>718</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>8</v>
@@ -6621,7 +6802,7 @@
         <v>766</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>8</v>
@@ -6638,10 +6819,10 @@
         <v>526</v>
       </c>
       <c r="D158" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>8</v>
@@ -6681,7 +6862,7 @@
         <v>735</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>8</v>
+        <v>967</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>8</v>
@@ -6741,7 +6922,7 @@
         <v>658</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>8</v>
@@ -6761,7 +6942,7 @@
         <v>755</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>8</v>
+        <v>1056</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>8</v>
@@ -6781,7 +6962,7 @@
         <v>574</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>8</v>
+        <v>1015</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>8</v>
@@ -6801,7 +6982,7 @@
         <v>720</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F166" s="1" t="s">
         <v>8</v>
@@ -6821,7 +7002,7 @@
         <v>681</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>8</v>
@@ -6838,10 +7019,10 @@
         <v>488</v>
       </c>
       <c r="D168" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>8</v>
+        <v>1010</v>
       </c>
       <c r="F168" s="1" t="s">
         <v>8</v>
@@ -6861,7 +7042,7 @@
         <v>673</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>8</v>
+        <v>988</v>
       </c>
       <c r="F169" s="1" t="s">
         <v>8</v>
@@ -6921,7 +7102,7 @@
         <v>672</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>8</v>
@@ -6941,7 +7122,7 @@
         <v>799</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>8</v>
@@ -6961,7 +7142,7 @@
         <v>706</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F174" s="1" t="s">
         <v>8</v>
@@ -6981,7 +7162,7 @@
         <v>796</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>8</v>
@@ -7001,7 +7182,7 @@
         <v>750</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>8</v>
@@ -7021,7 +7202,7 @@
         <v>759</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>8</v>
@@ -7041,7 +7222,7 @@
         <v>686</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>8</v>
+        <v>999</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>8</v>
@@ -7061,7 +7242,7 @@
         <v>659</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>8</v>
+        <v>1021</v>
       </c>
       <c r="F179" s="1" t="s">
         <v>8</v>
@@ -7081,7 +7262,7 @@
         <v>797</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>8</v>
+        <v>1059</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>8</v>
@@ -7101,7 +7282,7 @@
         <v>723</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>8</v>
+        <v>1005</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>8</v>
@@ -7121,7 +7302,7 @@
         <v>684</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>8</v>
+        <v>1026</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>8</v>
@@ -7141,7 +7322,7 @@
         <v>775</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>8</v>
+        <v>936</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>8</v>
@@ -7161,7 +7342,7 @@
         <v>779</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>8</v>
+        <v>946</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>8</v>
@@ -7181,7 +7362,7 @@
         <v>742</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>8</v>
+        <v>1048</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>8</v>
@@ -7201,7 +7382,7 @@
         <v>777</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>8</v>
@@ -7221,7 +7402,7 @@
         <v>771</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>8</v>
@@ -7241,7 +7422,7 @@
         <v>762</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="F188" s="1" t="s">
         <v>8</v>
@@ -7261,7 +7442,7 @@
         <v>688</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="F189" s="1" t="s">
         <v>8</v>
@@ -7281,7 +7462,7 @@
         <v>776</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>8</v>
+        <v>1011</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>8</v>
@@ -7301,7 +7482,7 @@
         <v>581</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>8</v>
+        <v>936</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>8</v>
@@ -7341,7 +7522,7 @@
         <v>751</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>8</v>
+        <v>1012</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>8</v>
@@ -7361,7 +7542,7 @@
         <v>639</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>8</v>
@@ -7381,7 +7562,7 @@
         <v>669</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>8</v>
+        <v>942</v>
       </c>
       <c r="F195" s="1" t="s">
         <v>8</v>
@@ -7401,7 +7582,7 @@
         <v>804</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>8</v>
+        <v>1002</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>8</v>
@@ -7421,7 +7602,7 @@
         <v>770</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>8</v>
+        <v>966</v>
       </c>
       <c r="F197" s="1" t="s">
         <v>8</v>
@@ -7441,7 +7622,7 @@
         <v>778</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F198" s="1" t="s">
         <v>8</v>
@@ -7461,7 +7642,7 @@
         <v>621</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>8</v>
+        <v>1016</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>8</v>
@@ -7481,7 +7662,7 @@
         <v>769</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>8</v>
+        <v>945</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>8</v>
@@ -7501,7 +7682,7 @@
         <v>772</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F201" s="1" t="s">
         <v>8</v>
@@ -7521,7 +7702,7 @@
         <v>773</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>8</v>
+        <v>949</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>8</v>
@@ -7541,7 +7722,7 @@
         <v>691</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>8</v>
+        <v>988</v>
       </c>
       <c r="F203" s="1" t="s">
         <v>8</v>
@@ -7561,7 +7742,7 @@
         <v>780</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>8</v>
+        <v>975</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>8</v>
@@ -7581,7 +7762,7 @@
         <v>618</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>8</v>
@@ -7601,7 +7782,7 @@
         <v>783</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F206" s="1" t="s">
         <v>8</v>
@@ -7621,7 +7802,7 @@
         <v>785</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>8</v>
+        <v>1035</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>8</v>
@@ -7641,7 +7822,7 @@
         <v>689</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F208" s="1" t="s">
         <v>8</v>
@@ -7661,7 +7842,7 @@
         <v>641</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>8</v>
@@ -7681,7 +7862,7 @@
         <v>753</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F210" s="1" t="s">
         <v>8</v>
@@ -7701,7 +7882,7 @@
         <v>748</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="F211" s="1" t="s">
         <v>8</v>
@@ -7721,7 +7902,7 @@
         <v>789</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>8</v>
@@ -7741,7 +7922,7 @@
         <v>791</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>8</v>
+        <v>991</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>8</v>
@@ -7761,7 +7942,7 @@
         <v>784</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>8</v>
+        <v>1028</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>8</v>
@@ -7781,7 +7962,7 @@
         <v>683</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>963</v>
+        <v>1017</v>
       </c>
       <c r="F215" s="1" t="s">
         <v>8</v>
@@ -7801,7 +7982,7 @@
         <v>747</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F216" s="1" t="s">
         <v>8</v>
@@ -7821,7 +8002,7 @@
         <v>660</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>8</v>
@@ -7841,7 +8022,7 @@
         <v>697</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>8</v>
+        <v>981</v>
       </c>
       <c r="F218" s="1" t="s">
         <v>8</v>
@@ -7881,7 +8062,7 @@
         <v>696</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>8</v>
+        <v>937</v>
       </c>
       <c r="F220" s="1" t="s">
         <v>8</v>
@@ -7901,7 +8082,7 @@
         <v>730</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>8</v>
@@ -7921,7 +8102,7 @@
         <v>798</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>8</v>
+        <v>966</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>8</v>
@@ -7941,7 +8122,7 @@
         <v>717</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>8</v>
+        <v>1052</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>8</v>
@@ -7961,7 +8142,7 @@
         <v>626</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>8</v>
+        <v>938</v>
       </c>
       <c r="F224" s="1" t="s">
         <v>8</v>
@@ -7981,7 +8162,7 @@
         <v>800</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>8</v>
+        <v>1003</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>8</v>
@@ -8001,7 +8182,7 @@
         <v>649</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>8</v>
+        <v>1043</v>
       </c>
       <c r="F226" s="1" t="s">
         <v>8</v>
@@ -8021,7 +8202,7 @@
         <v>739</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>8</v>
+        <v>1007</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>8</v>
@@ -8038,10 +8219,10 @@
         <v>504</v>
       </c>
       <c r="D228" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>8</v>
+        <v>962</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>8</v>
@@ -8081,7 +8262,7 @@
         <v>675</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="F230" s="1" t="s">
         <v>8</v>
@@ -8121,7 +8302,7 @@
         <v>711</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>8</v>
+        <v>951</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>8</v>
@@ -8138,7 +8319,7 @@
         <v>480</v>
       </c>
       <c r="D233" t="s">
-        <v>805</v>
+        <v>1001</v>
       </c>
       <c r="E233" s="1" t="s">
         <v>8</v>
@@ -8161,7 +8342,7 @@
         <v>648</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>8</v>
+        <v>1043</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>8</v>
@@ -8181,7 +8362,7 @@
         <v>749</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>8</v>
+        <v>998</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>8</v>
@@ -8201,7 +8382,7 @@
         <v>692</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>8</v>
+        <v>963</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>8</v>
@@ -8221,7 +8402,7 @@
         <v>656</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>8</v>
@@ -8238,10 +8419,10 @@
         <v>500</v>
       </c>
       <c r="D238" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>8</v>
+        <v>1010</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>8</v>
@@ -8261,7 +8442,7 @@
         <v>687</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>8</v>
@@ -8281,7 +8462,7 @@
         <v>676</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>8</v>
+        <v>1022</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>8</v>
@@ -8301,7 +8482,7 @@
         <v>733</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>8</v>
@@ -8321,7 +8502,7 @@
         <v>507</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>8</v>
@@ -8338,10 +8519,10 @@
         <v>512</v>
       </c>
       <c r="D243" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="F243" s="1" t="s">
         <v>8</v>
@@ -8358,10 +8539,10 @@
         <v>494</v>
       </c>
       <c r="D244" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>8</v>
+        <v>1005</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>8</v>
@@ -8378,10 +8559,10 @@
         <v>496</v>
       </c>
       <c r="D245" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>8</v>
@@ -8398,10 +8579,10 @@
         <v>498</v>
       </c>
       <c r="D246" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>8</v>
+        <v>987</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>8</v>
@@ -8418,10 +8599,10 @@
         <v>492</v>
       </c>
       <c r="D247" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>8</v>
+        <v>1037</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>8</v>
@@ -8438,10 +8619,10 @@
         <v>490</v>
       </c>
       <c r="D248" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>8</v>
+        <v>967</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>8</v>
@@ -8461,7 +8642,7 @@
         <v>582</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>8</v>
+        <v>1058</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>8</v>
@@ -8481,7 +8662,7 @@
         <v>640</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>8</v>
+        <v>1021</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>8</v>
@@ -8501,7 +8682,7 @@
         <v>653</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>8</v>
@@ -8521,7 +8702,7 @@
         <v>792</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>8</v>
+        <v>979</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>8</v>
@@ -8541,7 +8722,7 @@
         <v>690</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>8</v>
@@ -8561,7 +8742,7 @@
         <v>787</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>8</v>
+        <v>964</v>
       </c>
       <c r="F254" s="1" t="s">
         <v>8</v>
@@ -8601,7 +8782,7 @@
         <v>602</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>8</v>
+        <v>1002</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>8</v>
@@ -8621,7 +8802,7 @@
         <v>633</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F257" s="1" t="s">
         <v>8</v>
@@ -8661,7 +8842,7 @@
         <v>599</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>8</v>
+        <v>1047</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>8</v>
@@ -8681,7 +8862,7 @@
         <v>603</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>8</v>
+        <v>1033</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>8</v>
@@ -8701,7 +8882,7 @@
         <v>601</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F261" s="1" t="s">
         <v>8</v>
@@ -8721,7 +8902,7 @@
         <v>606</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>8</v>
@@ -8785,16 +8966,16 @@
         <v>533</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>905</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>906</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>907</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
@@ -8808,16 +8989,16 @@
         <v>534</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>908</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>909</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>910</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
@@ -8831,16 +9012,16 @@
         <v>535</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>890</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>891</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>892</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>8</v>
@@ -8854,16 +9035,16 @@
         <v>536</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>918</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>919</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>8</v>
@@ -8877,16 +9058,16 @@
         <v>537</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>888</v>
-      </c>
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>8</v>
@@ -8900,16 +9081,16 @@
         <v>538</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>911</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>912</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>913</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>914</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>8</v>
@@ -8923,16 +9104,16 @@
         <v>539</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>850</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>851</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>852</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>8</v>
@@ -8946,16 +9127,16 @@
         <v>540</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>866</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>867</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
@@ -8969,16 +9150,16 @@
         <v>541</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>903</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>904</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>8</v>
@@ -8992,16 +9173,16 @@
         <v>542</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>860</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>861</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>862</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>8</v>
@@ -9015,16 +9196,16 @@
         <v>543</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>840</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>8</v>
@@ -9038,16 +9219,16 @@
         <v>544</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>920</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>921</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>922</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>8</v>
@@ -9061,16 +9242,16 @@
         <v>545</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>843</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>8</v>
@@ -9084,16 +9265,16 @@
         <v>546</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>916</v>
-      </c>
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>8</v>
@@ -9107,16 +9288,16 @@
         <v>547</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>853</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>854</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>856</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>8</v>
@@ -9130,16 +9311,16 @@
         <v>548</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>857</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>858</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>859</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>8</v>
@@ -9153,16 +9334,16 @@
         <v>549</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>885</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>886</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>8</v>
@@ -9176,16 +9357,16 @@
         <v>550</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>873</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>874</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
@@ -9199,16 +9380,16 @@
         <v>551</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>8</v>
@@ -9222,16 +9403,16 @@
         <v>552</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>900</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>901</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
@@ -9245,16 +9426,16 @@
         <v>553</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>896</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>897</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>898</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>8</v>
@@ -9268,16 +9449,16 @@
         <v>554</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>923</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>924</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>925</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
@@ -9291,16 +9472,16 @@
         <v>555</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>926</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>927</v>
-      </c>
       <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>8</v>
@@ -9314,16 +9495,16 @@
         <v>556</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>847</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>848</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>849</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>8</v>
@@ -9337,16 +9518,16 @@
         <v>557</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>875</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>876</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>877</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>878</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>8</v>
@@ -9360,16 +9541,16 @@
         <v>558</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>879</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>880</v>
-      </c>
       <c r="E27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
@@ -9383,16 +9564,16 @@
         <v>559</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>895</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>8</v>
@@ -9406,16 +9587,16 @@
         <v>560</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>870</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>871</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>8</v>
@@ -9429,16 +9610,16 @@
         <v>561</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>837</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>8</v>
@@ -9452,16 +9633,16 @@
         <v>562</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>882</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>883</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>8</v>
@@ -9475,16 +9656,16 @@
         <v>563</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>928</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>929</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>930</v>
-      </c>
       <c r="F32" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>8</v>
@@ -9498,13 +9679,13 @@
         <v>564</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>931</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>932</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>8</v>
@@ -9521,13 +9702,13 @@
         <v>565</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>934</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>935</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>936</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>8</v>
@@ -9571,7 +9752,7 @@
         <v>567</v>
       </c>
       <c r="B2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -9579,7 +9760,7 @@
         <v>568</v>
       </c>
       <c r="B3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -9587,7 +9768,7 @@
         <v>569</v>
       </c>
       <c r="B4" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -9595,7 +9776,7 @@
         <v>570</v>
       </c>
       <c r="B5" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -9603,7 +9784,7 @@
         <v>571</v>
       </c>
       <c r="B6" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>